<commit_message>
NZ BOM updates for various hardware components
Update to include prices and links for purchases made
</commit_message>
<xml_diff>
--- a/BOM food computer (New Zealand).xlsx
+++ b/BOM food computer (New Zealand).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\GitHub\gro-hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raycooke/Documents/Projects/FoodComputer/gro-hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,20 @@
     <sheet name="Kit" sheetId="3" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
   <si>
     <t>Item Name</t>
   </si>
@@ -75,9 +83,6 @@
     <t>CyberPower CSB606 Surge Protector 6-Outlets 6-Ft Cord 900 Joules</t>
   </si>
   <si>
-    <t>Corrugated plastic, white, 0.157" thick, 48" x 96"</t>
-  </si>
-  <si>
     <t>plastic box</t>
   </si>
   <si>
@@ -102,24 +107,15 @@
     <t>12V 30A 360W Switching Power Supply for LED Strip Light</t>
   </si>
   <si>
-    <t>Hex bolts, 3/8"-16, 1 1/2" long</t>
-  </si>
-  <si>
     <t>motherboard panel to motherboard dock panel mounting</t>
   </si>
   <si>
-    <t>Hex bolts, 3/8"-16, 1" long</t>
-  </si>
-  <si>
     <t>PVC to punched angle connections</t>
   </si>
   <si>
     <t>C2G / Cables To Go 03137 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (1 Foot/0.30 Meters)</t>
   </si>
   <si>
-    <t>Hex bolts, 3/8"-16, 1/2" long</t>
-  </si>
-  <si>
     <t>punched angle to punched angle connections</t>
   </si>
   <si>
@@ -141,9 +137,6 @@
     <t>CanaKit 5V 2.5A Raspberry Pi 2 Power Supply (UL Listed)</t>
   </si>
   <si>
-    <t>Nuts, 3/8"-16</t>
-  </si>
-  <si>
     <t>back of each hex bolt</t>
   </si>
   <si>
@@ -153,15 +146,9 @@
     <t>window, side plate</t>
   </si>
   <si>
-    <t>Punched angle, 1 1/4" x 48"</t>
-  </si>
-  <si>
     <t>material for metal frame</t>
   </si>
   <si>
-    <t>Punched flat, 1 3/8", 36"</t>
-  </si>
-  <si>
     <t>LED panel mounting</t>
   </si>
   <si>
@@ -174,9 +161,6 @@
     <t>base board, motherboard panel, motherboard dock panel, feet</t>
   </si>
   <si>
-    <t>* link is to 48" x 96" because 24" x 96" is in stores but not online</t>
-  </si>
-  <si>
     <t>Reservoir bin</t>
   </si>
   <si>
@@ -186,9 +170,6 @@
     <t>Raspberry Pi 2 Model B Desktop (Quad Core CPU 900 MHz, 1 GB RAM, Linux)</t>
   </si>
   <si>
-    <t>Threaded rod, 3/8", 36"</t>
-  </si>
-  <si>
     <t>Kingston 8 GB microSDHC Class 4 Flash Memory Card SDC4/8GBET</t>
   </si>
   <si>
@@ -198,9 +179,6 @@
     <t>foam box</t>
   </si>
   <si>
-    <t>Washers, 3/8"</t>
-  </si>
-  <si>
     <t>for most bolt connections</t>
   </si>
   <si>
@@ -583,13 +561,61 @@
   </si>
   <si>
     <t>PRICE (NZD)</t>
+  </si>
+  <si>
+    <t>Corrugated plastic, white, 3mm thick, 1220 x 2440</t>
+  </si>
+  <si>
+    <t>Bunnings</t>
+  </si>
+  <si>
+    <t>Purchased by</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Not available online</t>
+  </si>
+  <si>
+    <t>Not available online - ALLSET 32L Storage Tub</t>
+  </si>
+  <si>
+    <t>Threaded rod, M6 1m</t>
+  </si>
+  <si>
+    <t>Washers, M6</t>
+  </si>
+  <si>
+    <t>Hex bolts, M6, 40mm long</t>
+  </si>
+  <si>
+    <t>Hex bolts, M6, 25mm long</t>
+  </si>
+  <si>
+    <t>Hex bolts, M6, 20mm long</t>
+  </si>
+  <si>
+    <t>Included in price of each bolt</t>
+  </si>
+  <si>
+    <t>Nuts, M6</t>
+  </si>
+  <si>
+    <t>Mitre10</t>
+  </si>
+  <si>
+    <t>Aluminium angle, 1.6 x 20 x 20 mm, 2.5m</t>
+  </si>
+  <si>
+    <t>Aluminium flat, 32 x 3 mm, 2m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -615,19 +641,7 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <u/>
-      <sz val="8"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -684,6 +698,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -714,10 +734,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -740,22 +761,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -763,16 +782,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -785,33 +804,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -873,9 +898,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -908,9 +933,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1092,21 +1117,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,13 +1145,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1136,7 +1161,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CyberPower-CSB606-Protector-6-Outlets-Joules/dp/B00FLTTGYG/ref=pd_sim_23_1?ie=UTF8&amp;refRID=163NC2W6A2KW7EF2RB9B","Power Strip")</f>
         <v>Power Strip</v>
@@ -1151,12 +1176,12 @@
         <v>1</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <f t="shared" ref="F3:F5" si="0">E3*D3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Switching-Power-Supply-Strip-Light/dp/B007MWNF5Q/ref=pd_sim_60_6?ie=UTF8&amp;refRID=0WA6QTYVKRWRGRG1ZKN2A","Main Power Supply")</f>
         <v>Main Power Supply</v>
@@ -1165,40 +1190,40 @@
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
       </c>
       <c r="E4" s="8"/>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>30</v>
+      <c r="C5" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1206,187 +1231,187 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CanaKit-Raspberry-Power-Supply-Listed/dp/B00MARDJZ4/ref=sr_1_2?ie=UTF8&amp;qid=1439988175&amp;sr=8-2&amp;keywords=raspberry+pi+2+power+supply","Raspberry Pi Power Supply")</f>
         <v>Raspberry Pi Power Supply</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="18">
+      <c r="C7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="16">
         <f t="shared" ref="F7:F11" si="1">E7*D7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Ximico-Arduino-Cable-Atmega2560-16au-Compatible/dp/B00KG3SBE8/ref=sr_1_2?s=pc&amp;ie=UTF8&amp;qid=1439935660&amp;sr=1-2&amp;keywords=arduino+mega","Arduino Mega 2560")</f>
         <v>Arduino Mega 2560</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="15">
-        <v>1</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18">
+      <c r="C8" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Raspberry-Pi-Model-Desktop-Linux/dp/B00T2U7R7I","Raspberry Pi 2 Model B")</f>
         <v>Raspberry Pi 2 Model B</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="15">
-        <v>1</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="18">
+      <c r="C9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_8?s=pc&amp;ie=UTF8&amp;qid=1439988385&amp;sr=1-8&amp;keywords=micro+SD","Micro SD Card")</f>
         <v>Micro SD Card</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="15">
-        <v>1</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="18">
+      <c r="C10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EUHRLF6/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1DCPNQKKEISZB","Ethernet cable")</f>
         <v>Ethernet cable</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="15">
-        <v>1</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="18">
+      <c r="C11" s="17"/>
+      <c r="D11" s="13">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Gikfun-Protoshield-Prototype-Shield-Arduino/dp/B00Q9YBQ04/ref=sr_1_6?s=pc&amp;ie=UTF8&amp;qid=1439935499&amp;sr=1-6&amp;keywords=protoshield","Arduino Mega Protoshield")</f>
         <v>Arduino Mega Protoshield</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="18">
+      <c r="C12" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="16">
         <f t="shared" ref="F12:F15" si="2">E12*D12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Base-Shield-V2-p-1378.html","Grove Base Shield")</f>
         <v>Grove Base Shield</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="15">
-        <v>1</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="18">
+      <c r="B13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="str">
         <f>HYPERLINK("https://www.adafruit.com/products/2097","Touchscreen Display")</f>
         <v>Touchscreen Display</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="18">
+      <c r="B14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/ribbon-cable-Raspberry-stackable-header/dp/B00G84WNA2/ref=sr_1_1?ie=UTF8&amp;qid=1440708449&amp;sr=8-1&amp;keywords=raspberry+pi+cable","GPIO Cable ")</f>
         <v xml:space="preserve">GPIO Cable </v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>68</v>
+      <c r="C15" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="18">
+      <c r="F15" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1394,109 +1419,109 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/JBtek-Channel-Module-Arduino-Raspberry/dp/B00KTEN3TM/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1439935182&amp;sr=1-1&amp;keywords=4+Channel+Relay","4-Channel Relay")</f>
         <v>4-Channel Relay</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="15">
+      <c r="C17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="13">
         <v>2</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="18">
+      <c r="E17" s="13"/>
+      <c r="F17" s="16">
         <f t="shared" ref="F17:F21" si="3">E17*D17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/52171-4E-Pre-Galvanized-Eccentric-Knockouts/dp/B000HEFCKC/ref=pd_bxgy_60_text_y","AC Relay Box Back Receptacle")</f>
         <v>AC Relay Box Back Receptacle</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="18">
+      <c r="C18" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/RS8-Outlet-Surface-Square-Galvanized/dp/B000HEIU9W/ref=pd_sim_60_23?ie=UTF8&amp;refRID=0C95J370DWVEWW0H1MG8","AC Relay Box Front Panel")</f>
         <v>AC Relay Box Front Panel</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="18">
+      <c r="C19" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Leviton-T5320-W-Resistant-Receptacle-Residential/dp/B0015R9M2Y/ref=pd_bxgy_60_img_z","AC Plug")</f>
         <v>AC Plug</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="15">
+      <c r="C20" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="13">
         <v>2</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="18">
+      <c r="E20" s="13"/>
+      <c r="F20" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>74</v>
+      <c r="C21" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="12">
+      <c r="F21" s="11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1504,7 +1529,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Triangle-Bulbs-T93007-Waterproof-Flexible/dp/B005EHHLD8/ref=sr_1_1?ie=UTF8&amp;qid=1443799060&amp;sr=8-1&amp;keywords=waterproof+led+strip","White LED Strip")</f>
         <v>White LED Strip</v>
@@ -1512,19 +1537,19 @@
       <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>76</v>
+      <c r="C23" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="D23" s="8">
         <v>2</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="12">
+      <c r="F23" s="11">
         <f t="shared" ref="F23:F24" si="4">E23*D23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Erligpowht-Indoor-Garden-Plant-Hanging/dp/B00S2DPYQM/ref=sr_1_fkmr2_2?ie=UTF8&amp;qid=1443799150&amp;sr=8-2-fkmr2&amp;keywords=grow+led+panel+erwl","Grow LED Panel")</f>
         <v>Grow LED Panel</v>
@@ -1532,21 +1557,21 @@
       <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>77</v>
+      <c r="C24" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="D24" s="8">
         <v>2</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="12">
+      <c r="F24" s="11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1554,47 +1579,47 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B003XDTWN2/ref=sr_ph?&amp;ie=UTF8&amp;qid=1440085101&amp;sr=1&amp;keywords=heater","Heater")</f>
         <v>Heater</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="15">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="18">
+      <c r="C26" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="16">
         <f t="shared" ref="F26:F31" si="5">E26*D26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Acoustic-Audio-Tek%C2%A8Portable-Humidifier-travel--White/dp/B00RM5Z44S/ref=sr_1_4?s=home-garden&amp;ie=UTF8&amp;qid=1440427700&amp;sr=1-4&amp;keywords=bottle+cap+humidifier","Humidifier")</f>
         <v>Humidifier</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="15">
-        <v>1</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="18">
+      <c r="C27" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="13">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B00WJW3NM4/ref=twister_B00WJW3M3Y?_encoding=UTF8&amp;psc=1","USB Wall Adapter")</f>
         <v>USB Wall Adapter</v>
@@ -1602,81 +1627,81 @@
       <c r="B28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>81</v>
+      <c r="C28" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="18">
+      <c r="F28" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Bgears-b-Blaster-120mm-Bearing-Extreme/dp/B0043GKY1W/ref=sr_1_1?ie=UTF8&amp;qid=1440020490&amp;sr=8-1&amp;keywords=bgears+120mm","Circulation/Vent Fans")</f>
         <v>Circulation/Vent Fans</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="15">
+      <c r="C29" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="13">
         <v>2</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="18">
+      <c r="E29" s="13"/>
+      <c r="F29" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Tjernlund-1519003-Wire-Fan-Guard/dp/B008RMKFTO/ref=sr_1_2?ie=UTF8&amp;qid=1440019946&amp;sr=8-2&amp;keywords=fan+guard","Fan Guards")</f>
         <v>Fan Guards</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="15">
+      <c r="C30" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="13">
         <v>2</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="18">
+      <c r="E30" s="13"/>
+      <c r="F30" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Dundas-Jafine-LC4WZW-ProVent-4-Inches/dp/B0016487CC/ref=sr_1_3?ie=UTF8&amp;qid=1440020385&amp;sr=8-3&amp;keywords=Louvered+Vent+Cap","Fan Louvres")</f>
         <v>Fan Louvres</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="15">
+      <c r="C31" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="13">
         <v>2</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="18">
+      <c r="E31" s="13"/>
+      <c r="F31" s="16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1684,67 +1709,67 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="str">
         <f>HYPERLINK("http://www.co2meter.com/products/cozir-0-2-co2-sensor","CO2 Sensor")</f>
         <v>CO2 Sensor</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="15">
-        <v>1</v>
-      </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="18">
+      <c r="B33" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="16">
         <f t="shared" ref="F33:F36" si="6">E33*D33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-TemperatureHumidity-Sensor-Pro-p-838.html","Air Temperature and Humidity Sensor")</f>
         <v>Air Temperature and Humidity Sensor</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="15">
-        <v>1</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="18">
+      <c r="B34" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="13">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-Digital-Light-Sensor-p-1281.html","Light Intensity Sensor")</f>
         <v>Light Intensity Sensor</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="15">
-        <v>1</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="18">
+      <c r="B35" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="13">
+        <v>1</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YCDHQ8K?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o06_s00","Webcam")</f>
         <v>Webcam</v>
@@ -1752,21 +1777,21 @@
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>90</v>
+      <c r="C36" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="D36" s="8">
         <v>1</v>
       </c>
       <c r="E36" s="8"/>
-      <c r="F36" s="18">
+      <c r="F36" s="16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1774,7 +1799,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009SUF08?keywords=reed%20switch&amp;qid=1443805349&amp;ref_=sr_1_1&amp;sr=8-1","Magnetic Switch")</f>
         <v>Magnetic Switch</v>
@@ -1783,40 +1808,40 @@
         <v>14</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D38" s="8">
         <v>1</v>
       </c>
       <c r="E38" s="8"/>
-      <c r="F38" s="18">
+      <c r="F38" s="16">
         <f t="shared" ref="F38:F39" si="7">E38*D38</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Micro-Limit-Switch-Roller-Action/dp/B00E0JOTV8/ref=sr_1_1?s=lamps-light&amp;ie=UTF8&amp;qid=1443805532&amp;sr=1-1&amp;keywords=limit+switch","Limit Switch")</f>
         <v>Limit Switch</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>94</v>
+        <v>83</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="D39" s="8">
         <v>1</v>
       </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="18">
+      <c r="F39" s="16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1824,109 +1849,109 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009YJ4N6?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Air Pump")</f>
         <v>Air Pump</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="15">
-        <v>1</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="18">
+      <c r="C41" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="13">
+        <v>1</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="16">
         <f t="shared" ref="F41:F45" si="8">E41*D41</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Jardin-Aquarium-Ceramic-Diffusers-Diameter/dp/B0050HJ7Q6/ref=pd_bxgy_199_img_z","Air Stone")</f>
         <v>Air Stone</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="15">
-        <v>1</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="18">
+      <c r="C42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Standard-Airline-Tubing-Accessories-25-Feet/dp/B0002563MW/ref=pd_bxgy_199_img_y","Air Pump Tubing")</f>
         <v>Air Pump Tubing</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="15">
-        <v>1</v>
-      </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="18">
+      <c r="C43" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EWENMAU?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_2&amp;smid=A14L9DIA3NK9B0","Aquarium Pump")</f>
         <v>Aquarium Pump</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>100</v>
+      <c r="B44" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="D44" s="8">
         <v>1</v>
       </c>
       <c r="E44" s="8"/>
-      <c r="F44" s="18">
+      <c r="F44" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0079QUTSQ?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Pump Tubing")</f>
         <v>Pump Tubing</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>101</v>
+      <c r="B45" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="D45" s="8">
         <v>1</v>
       </c>
       <c r="E45" s="8"/>
-      <c r="F45" s="18">
+      <c r="F45" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1934,49 +1959,49 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1123&amp;search=DFR0300#.VdTDoFNViko","Water Temperature and EC Sensor")</f>
         <v>Water Temperature and EC Sensor</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="15">
-        <v>1</v>
-      </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="18">
+      <c r="B47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47" s="13">
+        <v>1</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="16">
         <f t="shared" ref="F47:F48" si="9">E47*D47</f>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1025#.Vg60SBNViko","pH Sensor")</f>
         <v>pH Sensor</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="15">
-        <v>1</v>
-      </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="18">
+      <c r="B48" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="13">
+        <v>1</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1984,7 +2009,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00BL63ZU4?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","Cable Management Box")</f>
         <v>Cable Management Box</v>
@@ -1992,29 +2017,29 @@
       <c r="B50" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>107</v>
+      <c r="C50" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="D50" s="8">
         <v>1</v>
       </c>
       <c r="E50" s="8"/>
-      <c r="F50" s="18">
+      <c r="F50" s="16">
         <f>E50*D50</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="19"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2022,27 +2047,27 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="str">
         <f>HYPERLINK("C2G / Cables To Go 53408 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (12 Feet/3.65 Meters)","Sacrificial AC Extension Cable for high gauge wire")</f>
         <v>Sacrificial AC Extension Cable for high gauge wire</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="15" t="s">
-        <v>109</v>
+      <c r="C53" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="D53" s="8">
         <v>1</v>
       </c>
       <c r="E53" s="8"/>
-      <c r="F53" s="12">
+      <c r="F53" s="11">
         <f t="shared" ref="F53:F55" si="10">E53*D53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Wago-222-412-222-413-Lever-Nut-Assortment/dp/B00U4520JK/ref=sr_1_1?ie=UTF8&amp;qid=1443798480&amp;sr=8-1&amp;keywords=wago+lever+nut+assortment","Wago Lever Nut Assortment")</f>
         <v>Wago Lever Nut Assortment</v>
@@ -2050,178 +2075,178 @@
       <c r="B54" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>110</v>
+      <c r="C54" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="D54" s="8">
         <v>1</v>
       </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="12">
+      <c r="F54" s="11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Vktech-150pcs-Shrink-Tubing-Sleeving/dp/B00EXLPLTW/ref=sr_1_2?ie=UTF8&amp;qid=1440019080&amp;sr=8-2&amp;keywords=vktech+heat+shrink","Heat Shrink Tubing")</f>
         <v>Heat Shrink Tubing</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="15">
-        <v>1</v>
-      </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="18">
+      <c r="C55" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="13">
+        <v>1</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-c-98_106_57/?ref=crumb","Grove Cables")</f>
         <v>Grove Cables</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
+        <v>102</v>
+      </c>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="24" t="str">
+        <v>103</v>
+      </c>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/3M-Scotch-1-in-x-12-5-yds-Indoor-Outdoor-Mounting-Tape-411-LONG-DC/100153200","Foam mounting tape")</f>
         <v>Foam mounting tape</v>
       </c>
-      <c r="B58" s="25" t="s">
-        <v>114</v>
+      <c r="B58" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D58" s="8">
         <v>1</v>
       </c>
       <c r="E58" s="8"/>
-      <c r="F58" s="18">
+      <c r="F58" s="16">
         <f t="shared" ref="F58:F62" si="11">E58*D58</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="24" t="str">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" s="22" t="str">
         <f>HYPERLINK("http://www.amazon.com/3M-Electrical-75-Inch-66-Foot-0085-Inch/dp/B00004WCCP/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1443807012&amp;sr=1-1&amp;keywords=electrical+tape","Electrical Tape")</f>
         <v>Electrical Tape</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D59" s="8">
         <v>1</v>
       </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="18">
+      <c r="F59" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="str">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" s="22" t="str">
         <f>HYPERLINK("http://www.digikey.com/product-search/en?KeyWords=377-2132-ND&amp;WT.z_header=search_go","Air Exchange Box")</f>
         <v>Air Exchange Box</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D60" s="8">
         <v>1</v>
       </c>
       <c r="E60" s="8"/>
-      <c r="F60" s="18">
+      <c r="F60" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="24" t="str">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-6-x-1-2-in-Stainless-Steel-Pan-Head-Phillips-Sheet-Metal-Screw-50-per-Pack-800162/204275035","Short Screws")</f>
         <v>Short Screws</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>119</v>
+        <v>104</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="D61" s="8">
         <v>1</v>
       </c>
       <c r="E61" s="8"/>
-      <c r="F61" s="18">
+      <c r="F61" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="24" t="str">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-8-x-2-in-Zinc-Plated-Pan-Head-Phillips-Drive-Sheet-Metal-Screw-50-Piece-801632/204275094","Long Screws")</f>
         <v>Long Screws</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>120</v>
+        <v>104</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="D62" s="8">
         <v>1</v>
       </c>
       <c r="E62" s="8"/>
-      <c r="F62" s="18">
+      <c r="F62" s="16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
-      <c r="D63" s="26">
+      <c r="D63" s="24">
         <f>SUM(D2:D62)</f>
         <v>54</v>
       </c>
-      <c r="E63" s="27">
+      <c r="E63" s="25">
         <f>SUM(F2:F62)</f>
         <v>0</v>
       </c>
-      <c r="F63" s="26">
+      <c r="F63" s="24">
         <f>SUM(F2:F62)</f>
         <v>0</v>
       </c>
@@ -2233,24 +2258,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G21"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="181" zoomScalePageLayoutView="181" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2270,13 +2297,16 @@
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="H1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2289,554 +2319,546 @@
       <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="str">
-        <f>HYPERLINK("http://www.lowes.com/pd_11288-1638-1AG2196A___?productId=3502046&amp;pl=1&amp;Ntt=.22+acrylic+sheet","Lowe's")</f>
-        <v>Lowe's</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="4"/>
+      <c r="G2" s="46"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Coroplast-48-in-x-96-in-x-0-157-in-White-Corrugated-Plastic-Sheet-CP4896S/205351385","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E3" s="44" t="s">
+        <v>178</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G3" s="46">
+        <v>29.52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Project-Panels-2-ft-x-2-ft-Project-Panel-PP1/203553730?keyword=foam+project+panel","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E4" s="44" t="s">
+        <v>178</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G4" s="46">
+        <v>15.13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D5" s="4">
         <v>6</v>
       </c>
-      <c r="E5" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-2-in-Self-Adhesive-Anti-Skid-Surface-Pads-8-per-Pack-49971/203661153","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F5" s="4">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+      <c r="G5" s="46"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="13">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Rust-Oleum-Specialty-11-oz-Frosted-Glass-Spray-Paint-1903830/100195608","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F6" s="13">
-        <v>1</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="46"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-3-8-in-16-tpi-x-1-1-2-in-Stainless-Steel-Hex-Bolt-804316/204633369","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E7" t="s">
+        <v>178</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="46">
+        <f>6*0.43</f>
+        <v>2.58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4">
         <v>26</v>
       </c>
-      <c r="E8" s="10" t="str">
-        <f>HYPERLINK("http://www.mcmaster.com/#92240a624/=z8h0sm","McMaster")</f>
-        <v>McMaster</v>
+      <c r="E8" t="s">
+        <v>178</v>
       </c>
       <c r="F8" s="4">
-        <v>25</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="46">
+        <f>0.37*30</f>
+        <v>11.1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>31</v>
+        <v>187</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4">
         <v>46</v>
       </c>
-      <c r="E9" s="10" t="str">
-        <f>HYPERLINK("http://www.mcmaster.com/#92240a619/=z8h0yk","McMaster")</f>
-        <v>McMaster</v>
+      <c r="E9" t="s">
+        <v>178</v>
       </c>
       <c r="F9" s="4">
-        <v>25</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="G9" s="46">
+        <v>9.49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>180</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Loctite-13-5-oz-High-Performance-Spray-Adhesive-1408028/202365672","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="46"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" s="4">
         <v>44</v>
       </c>
-      <c r="E11" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/MASTER-MAGNETICS-0-7-in-Neodymium-Rare-Earth-Magnet-Discs-3-per-Pack-07047HD/202526369","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F11" s="4">
-        <v>3</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="4"/>
+      <c r="G11" s="46"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4">
         <v>83</v>
       </c>
-      <c r="E12" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-3-8-in-16-tpi-Zinc-Plated-Hex-Nut-100-Piece-per-Box-801750/204274086","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E12" t="s">
+        <v>178</v>
       </c>
       <c r="F12" s="4">
-        <v>100</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="46">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>180</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/LEXAN-48-in-x-36-in-x-093-in-Polycarbonate-Sheet-GE-38/202038065","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="4"/>
+      <c r="G13" s="46"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4">
-        <v>10</v>
-      </c>
-      <c r="E14" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Crown-Bolt-1-1-4-in-x-48-in-Zinc-Plated-Punched-Angle-41790/202183466","Home Depot")</f>
-        <v>Home Depot</v>
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>190</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14" s="46">
+        <f>12.55*5</f>
+        <v>62.75</v>
+      </c>
+      <c r="H14" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>45</v>
+        <v>192</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="13">
-        <v>2</v>
-      </c>
-      <c r="E15" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-1-3-8-in-x-36-in-Zinc-Plated-Punch-Flat-Bar-800337/204325640","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F15" s="13">
-        <v>1</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>190</v>
+      </c>
+      <c r="F15" s="12">
+        <v>1</v>
+      </c>
+      <c r="G15" s="46">
+        <v>25.88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
       </c>
-      <c r="E16" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Veranda-HP-1-2-in-x-48-in-x-8-ft-White-PVC-Trim-H120AWS6/205309788","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="4"/>
+      <c r="G16" s="46"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="10" t="str">
-        <f>HYPERLINK("http://www.amazon.com/gp/product/B000BC5EP8?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o02_s00","Amazon Prime")</f>
-        <v>Amazon Prime</v>
+      <c r="E17" t="s">
+        <v>178</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="46">
+        <v>9.98</v>
+      </c>
+      <c r="H17" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
       </c>
-      <c r="E18" s="14" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Crown-Bolt-3-8-in-x-36-in-Zinc-Threaded-Rod-17340/202183465","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E18" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="46">
+        <v>5.97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>180</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Super-TUFF-R-1-in-x-4-ft-x-8-ft-R-6-5-Insulating-Sheathing-268426/100322374","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="4"/>
+      <c r="G19" s="46"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>58</v>
+        <v>184</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4">
         <v>84</v>
       </c>
-      <c r="E20" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Crown-Bolt-3-8-in-Zinc-Plated-Cut-Washer-100-per-Box-46060/203639706","Home Depot")</f>
-        <v>Home Depot</v>
+      <c r="E20" t="s">
+        <v>178</v>
       </c>
       <c r="F20" s="4">
-        <v>100</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="G20" s="46">
+        <f>3.14*2</f>
+        <v>6.28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>180</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D21" s="4">
         <v>2</v>
       </c>
-      <c r="E21" s="10" t="str">
-        <f>HYPERLINK("http://www.homedepot.com/p/Frost-King-E-O-9-16-in-x-5-16-in-x-10-ft-Gray-EPDM-Cellular-Rubber-Weatherstrip-Tape-V27GA/100546771","Home Depot")</f>
-        <v>Home Depot</v>
-      </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="G21" s="46"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="20">
+        <v>52</v>
+      </c>
+      <c r="G22" s="46">
         <f>SUM(G2:G21)</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-    </row>
-    <row r="33" spans="6:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+        <v>178.67999999999998</v>
+      </c>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="6:7" ht="13" x14ac:dyDescent="0.15">
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="http://www.lowes.com/pd_11288-1638-1AG2196A___?productId=3502046&amp;pl=1&amp;Ntt=.22+acrylic+sheet"/>
-    <hyperlink ref="E3" r:id="rId2" display="http://www.homedepot.com/p/Coroplast-48-in-x-96-in-x-0-157-in-White-Corrugated-Plastic-Sheet-CP4896S/205351385"/>
-    <hyperlink ref="E4" r:id="rId3" display="http://www.homedepot.com/p/Project-Panels-2-ft-x-2-ft-Project-Panel-PP1/203553730?keyword=foam+project+panel"/>
-    <hyperlink ref="E5" r:id="rId4" display="http://www.homedepot.com/p/Everbilt-2-in-Self-Adhesive-Anti-Skid-Surface-Pads-8-per-Pack-49971/203661153"/>
-    <hyperlink ref="E6" r:id="rId5" display="http://www.homedepot.com/p/Rust-Oleum-Specialty-11-oz-Frosted-Glass-Spray-Paint-1903830/100195608"/>
-    <hyperlink ref="E7" r:id="rId6" display="http://www.homedepot.com/p/Everbilt-3-8-in-16-tpi-x-1-1-2-in-Stainless-Steel-Hex-Bolt-804316/204633369"/>
-    <hyperlink ref="E8" r:id="rId7" location="92240a624/=z8h0sm" display="http://www.mcmaster.com/ - 92240a624/=z8h0sm"/>
-    <hyperlink ref="E9" r:id="rId8" location="92240a619/=z8h0yk" display="http://www.mcmaster.com/ - 92240a619/=z8h0yk"/>
-    <hyperlink ref="E10" r:id="rId9" display="http://www.homedepot.com/p/Loctite-13-5-oz-High-Performance-Spray-Adhesive-1408028/202365672"/>
-    <hyperlink ref="E11" r:id="rId10" display="http://www.homedepot.com/p/MASTER-MAGNETICS-0-7-in-Neodymium-Rare-Earth-Magnet-Discs-3-per-Pack-07047HD/202526369"/>
-    <hyperlink ref="E12" r:id="rId11" display="http://www.homedepot.com/p/Everbilt-3-8-in-16-tpi-Zinc-Plated-Hex-Nut-100-Piece-per-Box-801750/204274086"/>
-    <hyperlink ref="E13" r:id="rId12" display="http://www.homedepot.com/p/LEXAN-48-in-x-36-in-x-093-in-Polycarbonate-Sheet-GE-38/202038065"/>
-    <hyperlink ref="E14" r:id="rId13" display="http://www.homedepot.com/p/Crown-Bolt-1-1-4-in-x-48-in-Zinc-Plated-Punched-Angle-41790/202183466"/>
-    <hyperlink ref="E15" r:id="rId14" display="http://www.homedepot.com/p/Everbilt-1-3-8-in-x-36-in-Zinc-Plated-Punch-Flat-Bar-800337/204325640"/>
-    <hyperlink ref="E16" r:id="rId15" display="http://www.homedepot.com/p/Veranda-HP-1-2-in-x-48-in-x-8-ft-White-PVC-Trim-H120AWS6/205309788"/>
-    <hyperlink ref="E17" r:id="rId16" display="http://www.amazon.com/gp/product/B000BC5EP8?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o02_s00"/>
-    <hyperlink ref="E18" r:id="rId17" display="http://www.homedepot.com/p/Crown-Bolt-3-8-in-x-36-in-Zinc-Threaded-Rod-17340/202183465"/>
-    <hyperlink ref="E19" r:id="rId18" display="http://www.homedepot.com/p/Super-TUFF-R-1-in-x-4-ft-x-8-ft-R-6-5-Insulating-Sheathing-268426/100322374"/>
-    <hyperlink ref="E20" r:id="rId19" display="http://www.homedepot.com/p/Crown-Bolt-3-8-in-Zinc-Plated-Cut-Washer-100-per-Box-46060/203639706"/>
-    <hyperlink ref="E21" r:id="rId20" display="http://www.homedepot.com/p/Frost-King-E-O-9-16-in-x-5-16-in-x-10-ft-Gray-EPDM-Cellular-Rubber-Weatherstrip-Tape-V27GA/100546771"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2846,23 +2868,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2882,436 +2904,436 @@
         <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="H1" s="5"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28">
-        <v>1</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="28">
-        <v>1</v>
-      </c>
-      <c r="E2" s="29" t="str">
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="26">
+        <v>1</v>
+      </c>
+      <c r="E2" s="27" t="str">
         <f>HYPERLINK("http://www.amazon.com/General-Hydroponics-GH1514-Control-Kit/dp/B000BNKWZY/ref=sr_1_5?s=lawn-garden&amp;ie=UTF8&amp;qid=1443817989&amp;sr=1-5&amp;keywords=general+hydroponics","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F2" s="28">
-        <v>1</v>
-      </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+      <c r="F2" s="26">
+        <v>1</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="32">
-        <v>1</v>
-      </c>
-      <c r="E3" s="29" t="str">
+      <c r="B3" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="30">
+        <v>1</v>
+      </c>
+      <c r="E3" s="27" t="str">
         <f t="shared" ref="E3:E4" si="0">HYPERLINK("http://www.jrpeters.com/Products/Hydroponics/Buy-Hydroponics.html","JRPeters")</f>
         <v>JRPeters</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28">
+      <c r="F3" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="32">
-        <v>1</v>
-      </c>
-      <c r="E4" s="29" t="str">
+      <c r="B4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="30">
+        <v>1</v>
+      </c>
+      <c r="E4" s="27" t="str">
         <f t="shared" si="0"/>
         <v>JRPeters</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28">
+      <c r="F4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="32">
-        <v>1</v>
-      </c>
-      <c r="E5" s="33" t="str">
+      <c r="B5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="30">
+        <v>1</v>
+      </c>
+      <c r="E5" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Clean-Ones-Disposable-Essentials-Latex-free/dp/B00D8I346S/ref=sr_1_1?ie=UTF8&amp;qid=1440429335&amp;sr=8-1&amp;keywords=latex+free+gloves+one+size","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28">
+      <c r="F5" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="32">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33" t="str">
+      <c r="B6" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="30">
+        <v>1</v>
+      </c>
+      <c r="E6" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Pyramex-S4110SMP-Safety-Glasses-Intruder/dp/B002KA00KS/ref=sr_1_2?ie=UTF8&amp;qid=1440429198&amp;sr=8-2&amp;keywords=safety+glasses","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="30">
         <v>6</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+      <c r="G6" s="30"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" s="32">
+      <c r="B7" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="30">
         <v>10</v>
       </c>
-      <c r="E7" s="33" t="str">
+      <c r="E7" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B005IQTSE0/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1EHJTTD3AJH1J","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="30">
         <v>100</v>
       </c>
-      <c r="G7" s="32"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28">
+      <c r="G7" s="30"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="32">
-        <v>1</v>
-      </c>
-      <c r="E8" s="33" t="str">
+      <c r="B8" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="30">
+        <v>1</v>
+      </c>
+      <c r="E8" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Fleischmanns-Active-Yeast-0-75-Packet/dp/B0014CTFU4/ref=sr_1_cc_1?s=aps&amp;ie=UTF8&amp;qid=1445014924&amp;sr=1-1-catcorr&amp;keywords=yeast+packets","Amazon  ")</f>
         <v xml:space="preserve">Amazon  </v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28">
+      <c r="G8" s="30"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>172</v>
-      </c>
-      <c r="D9" s="32">
-        <v>1</v>
-      </c>
-      <c r="E9" s="33" t="str">
+      <c r="B9" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="30">
+        <v>1</v>
+      </c>
+      <c r="E9" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Domino-Sugar-Granulated-10-Pound-Bags/dp/B00060N5OW/ref=sr_1_2?s=grocery&amp;ie=UTF8&amp;qid=1445014968&amp;sr=1-2&amp;keywords=sugar","Amazon")</f>
         <v>Amazon</v>
       </c>
-      <c r="F9" s="32">
-        <v>1</v>
-      </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28">
+      <c r="F9" s="30">
+        <v>1</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10" s="32">
+      <c r="B10" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="30">
         <v>6</v>
       </c>
-      <c r="E10" s="33" t="str">
+      <c r="E10" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YQLI1KK?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o02_s01","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="30">
         <v>10</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28">
+      <c r="G10" s="30"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="E11" s="33" t="str">
+      <c r="B11" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Watts-SVGE10-Pre-Cut-Diameter-10-Foot/dp/B000HE5DUG/ref=pd_sim_60_4?ie=UTF8&amp;refRID=09WC8C60A2AF6W59DZM7&amp;dpID=41P%2BeRnccFL&amp;dpSrc=sims&amp;preST=_AC_UL160_SR160%2C160_","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F11" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="G11" s="32"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28">
+      <c r="F11" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="32">
-        <v>1</v>
-      </c>
-      <c r="E12" s="33" t="str">
+      <c r="B12" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="30">
+        <v>1</v>
+      </c>
+      <c r="E12" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Inside-Diameter-Plastic-One-way-Check/dp/B005OUKJ1Q/ref=sr_1_1?ie=UTF8&amp;qid=1440704334&amp;sr=8-1&amp;keywords=one+way+valve&amp;pebp=1440704341610&amp;perid=18B8N4679WXNCNNQVW2B","Amazon  ")</f>
         <v xml:space="preserve">Amazon  </v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="30">
         <v>4</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28">
+      <c r="G12" s="30"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="D13" s="32">
-        <v>1</v>
-      </c>
-      <c r="E13" s="33" t="str">
+      <c r="B13" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1</v>
+      </c>
+      <c r="E13" s="31" t="str">
         <f>HYPERLINK("http://www.amazon.com/Grodan-Rockwool-Stonewool-Cuttings-Propagation/dp/B0087SJ3U0/ref=sr_1_1?ie=UTF8&amp;qid=1440422481&amp;sr=8-1&amp;keywords=horticubes","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="30">
         <v>200</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36">
+      <c r="G13" s="30"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="34">
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="D14" s="36">
-        <v>1</v>
-      </c>
-      <c r="E14" s="38" t="str">
+      <c r="B14" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="34">
+        <v>1</v>
+      </c>
+      <c r="E14" s="36" t="str">
         <f>HYPERLINK("http://www.amazon.com/Good-Cook-Classic-Plastic-Measuring/dp/B000BQKVQ6/ref=sr_1_cc_2?s=aps&amp;ie=UTF8&amp;qid=1445015255&amp;sr=1-2-catcorr&amp;keywords=plastic+measuring+spoons","Amazon Prime")</f>
         <v>Amazon Prime</v>
       </c>
-      <c r="F14" s="36">
-        <v>1</v>
-      </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="40">
+      <c r="F14" s="34">
+        <v>1</v>
+      </c>
+      <c r="G14" s="34"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="38">
         <f>SUM(G2:G14)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3341,255 +3363,255 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="40"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B3" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C3" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="42"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B4" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="40"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+      <c r="B5" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="40"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="40"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="40"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="40"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="40"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="42"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="40"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="42"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="40"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="42"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="40"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="40"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="40"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="40"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="43" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="40"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="40"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="42"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="43" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="40"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="42"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="42"/>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="40"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="41" t="s">
         <v>158</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="42"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="42"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="40"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="42"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="42"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="42"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="42"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="40"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="10"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="10"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="10"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="10"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A30" s="10"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated NZ BOM for magnets
Updated NZ BOM for magnets
</commit_message>
<xml_diff>
--- a/BOM food computer (New Zealand).xlsx
+++ b/BOM food computer (New Zealand).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22300" windowHeight="14680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="195">
   <si>
     <t>Item Name</t>
   </si>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>Aluminium flat, 32 x 3 mm, 2m</t>
+  </si>
+  <si>
+    <t>Magnetic Magnets</t>
+  </si>
+  <si>
+    <t>have gone for lower strength magnets than specified originally (to reduce cost) - will have to wait and see on the results! Cost includes shipping</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +2267,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="181" zoomScalePageLayoutView="181" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2270,11 +2276,11 @@
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2529,9 +2535,22 @@
       <c r="D11" s="4">
         <v>44</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="46"/>
-      <c r="I11" s="10"/>
+      <c r="E11" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="F11" s="4">
+        <v>36</v>
+      </c>
+      <c r="G11" s="46">
+        <f>2*25.9+5.9</f>
+        <v>57.699999999999996</v>
+      </c>
+      <c r="H11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
@@ -2788,7 +2807,7 @@
       </c>
       <c r="G22" s="46">
         <f>SUM(G2:G21)</f>
-        <v>178.67999999999998</v>
+        <v>236.37999999999997</v>
       </c>
       <c r="I22" s="10"/>
     </row>
@@ -2859,6 +2878,7 @@
     <hyperlink ref="E4" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BOM NZ edition
</commit_message>
<xml_diff>
--- a/BOM food computer (New Zealand).xlsx
+++ b/BOM food computer (New Zealand).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raycooke/Documents/Projects/FoodComputer/gro-hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22300" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -17,20 +17,17 @@
     <sheet name="Kit" sheetId="3" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="202">
   <si>
     <t>Item Name</t>
   </si>
@@ -633,13 +630,16 @@
   </si>
   <si>
     <t>Purchased By</t>
+  </si>
+  <si>
+    <t>Ash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -728,8 +728,15 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,6 +755,11 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -758,11 +770,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -861,8 +874,18 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1144,21 +1167,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1204,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1190,8 +1213,9 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CyberPower-CSB606-Protector-6-Outlets-Joules/dp/B00FLTTGYG/ref=pd_sim_23_1?ie=UTF8&amp;refRID=163NC2W6A2KW7EF2RB9B","Power Strip")</f>
         <v>Power Strip</v>
@@ -1210,8 +1234,11 @@
         <f t="shared" ref="F3:F5" si="0">E3*D3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G3" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Switching-Power-Supply-Strip-Light/dp/B007MWNF5Q/ref=pd_sim_60_6?ie=UTF8&amp;refRID=0WA6QTYVKRWRGRG1ZKN2A","Main Power Supply")</f>
         <v>Main Power Supply</v>
@@ -1230,8 +1257,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G4" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1250,8 +1280,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G5" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1260,8 +1293,9 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G6" s="48"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CanaKit-Raspberry-Power-Supply-Listed/dp/B00MARDJZ4/ref=sr_1_2?ie=UTF8&amp;qid=1439988175&amp;sr=8-2&amp;keywords=raspberry+pi+2+power+supply","Raspberry Pi Power Supply")</f>
         <v>Raspberry Pi Power Supply</v>
@@ -1280,8 +1314,11 @@
         <f t="shared" ref="F7:F11" si="1">E7*D7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G7" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Ximico-Arduino-Cable-Atmega2560-16au-Compatible/dp/B00KG3SBE8/ref=sr_1_2?s=pc&amp;ie=UTF8&amp;qid=1439935660&amp;sr=1-2&amp;keywords=arduino+mega","Arduino Mega 2560")</f>
         <v>Arduino Mega 2560</v>
@@ -1300,8 +1337,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G8" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Raspberry-Pi-Model-Desktop-Linux/dp/B00T2U7R7I","Raspberry Pi 2 Model B")</f>
         <v>Raspberry Pi 2 Model B</v>
@@ -1320,8 +1360,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G9" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_8?s=pc&amp;ie=UTF8&amp;qid=1439988385&amp;sr=1-8&amp;keywords=micro+SD","Micro SD Card")</f>
         <v>Micro SD Card</v>
@@ -1340,8 +1383,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G10" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EUHRLF6/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1DCPNQKKEISZB","Ethernet cable")</f>
         <v>Ethernet cable</v>
@@ -1358,8 +1404,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G11" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Gikfun-Protoshield-Prototype-Shield-Arduino/dp/B00Q9YBQ04/ref=sr_1_6?s=pc&amp;ie=UTF8&amp;qid=1439935499&amp;sr=1-6&amp;keywords=protoshield","Arduino Mega Protoshield")</f>
         <v>Arduino Mega Protoshield</v>
@@ -1378,8 +1427,11 @@
         <f t="shared" ref="F12:F15" si="2">E12*D12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G12" s="49" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Base-Shield-V2-p-1378.html","Grove Base Shield")</f>
         <v>Grove Base Shield</v>
@@ -1398,8 +1450,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G13" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
         <f>HYPERLINK("https://www.adafruit.com/products/2097","Touchscreen Display")</f>
         <v>Touchscreen Display</v>
@@ -1418,8 +1473,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G14" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/ribbon-cable-Raspberry-stackable-header/dp/B00G84WNA2/ref=sr_1_1?ie=UTF8&amp;qid=1440708449&amp;sr=8-1&amp;keywords=raspberry+pi+cable","GPIO Cable ")</f>
         <v xml:space="preserve">GPIO Cable </v>
@@ -1438,8 +1496,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G15" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1449,7 +1510,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/JBtek-Channel-Module-Arduino-Raspberry/dp/B00KTEN3TM/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1439935182&amp;sr=1-1&amp;keywords=4+Channel+Relay","4-Channel Relay")</f>
         <v>4-Channel Relay</v>
@@ -1468,8 +1529,11 @@
         <f t="shared" ref="F17:F21" si="3">E17*D17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G17" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/52171-4E-Pre-Galvanized-Eccentric-Knockouts/dp/B000HEFCKC/ref=pd_bxgy_60_text_y","AC Relay Box Back Receptacle")</f>
         <v>AC Relay Box Back Receptacle</v>
@@ -1488,8 +1552,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G18" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/RS8-Outlet-Surface-Square-Galvanized/dp/B000HEIU9W/ref=pd_sim_60_23?ie=UTF8&amp;refRID=0C95J370DWVEWW0H1MG8","AC Relay Box Front Panel")</f>
         <v>AC Relay Box Front Panel</v>
@@ -1508,8 +1575,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G19" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>199</v>
       </c>
@@ -1527,8 +1597,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G20" s="50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>198</v>
       </c>
@@ -1546,8 +1619,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G21" s="50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1557,14 +1633,14 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="54" t="s">
         <v>66</v>
       </c>
       <c r="D23" s="8">
@@ -1575,8 +1651,11 @@
         <f t="shared" ref="F23:F24" si="4">E23*D23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G23" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="47" t="s">
         <v>196</v>
       </c>
@@ -1600,7 +1679,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
@@ -1610,7 +1689,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B003XDTWN2/ref=sr_ph?&amp;ie=UTF8&amp;qid=1440085101&amp;sr=1&amp;keywords=heater","Heater")</f>
         <v>Heater</v>
@@ -1629,8 +1708,11 @@
         <f t="shared" ref="F26:F31" si="5">E26*D26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="G26" s="51" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Acoustic-Audio-Tek%C2%A8Portable-Humidifier-travel--White/dp/B00RM5Z44S/ref=sr_1_4?s=home-garden&amp;ie=UTF8&amp;qid=1440427700&amp;sr=1-4&amp;keywords=bottle+cap+humidifier","Humidifier")</f>
         <v>Humidifier</v>
@@ -1649,8 +1731,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G27" s="51" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B00WJW3NM4/ref=twister_B00WJW3M3Y?_encoding=UTF8&amp;psc=1","USB Wall Adapter")</f>
         <v>USB Wall Adapter</v>
@@ -1670,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Bgears-b-Blaster-120mm-Bearing-Extreme/dp/B0043GKY1W/ref=sr_1_1?ie=UTF8&amp;qid=1440020490&amp;sr=8-1&amp;keywords=bgears+120mm","Circulation/Vent Fans")</f>
         <v>Circulation/Vent Fans</v>
@@ -1689,8 +1774,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G29" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Tjernlund-1519003-Wire-Fan-Guard/dp/B008RMKFTO/ref=sr_1_2?ie=UTF8&amp;qid=1440019946&amp;sr=8-2&amp;keywords=fan+guard","Fan Guards")</f>
         <v>Fan Guards</v>
@@ -1709,8 +1797,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G30" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Dundas-Jafine-LC4WZW-ProVent-4-Inches/dp/B0016487CC/ref=sr_1_3?ie=UTF8&amp;qid=1440020385&amp;sr=8-3&amp;keywords=Louvered+Vent+Cap","Fan Louvres")</f>
         <v>Fan Louvres</v>
@@ -1729,8 +1820,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G31" s="53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -1740,7 +1834,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="str">
         <f>HYPERLINK("http://www.co2meter.com/products/cozir-0-2-co2-sensor","CO2 Sensor")</f>
         <v>CO2 Sensor</v>
@@ -1760,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-TemperatureHumidity-Sensor-Pro-p-838.html","Air Temperature and Humidity Sensor")</f>
         <v>Air Temperature and Humidity Sensor</v>
@@ -1780,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-Digital-Light-Sensor-p-1281.html","Light Intensity Sensor")</f>
         <v>Light Intensity Sensor</v>
@@ -1800,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YCDHQ8K?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o06_s00","Webcam")</f>
         <v>Webcam</v>
@@ -1820,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
@@ -1830,7 +1924,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009SUF08?keywords=reed%20switch&amp;qid=1443805349&amp;ref_=sr_1_1&amp;sr=8-1","Magnetic Switch")</f>
         <v>Magnetic Switch</v>
@@ -1850,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Micro-Limit-Switch-Roller-Action/dp/B00E0JOTV8/ref=sr_1_1?s=lamps-light&amp;ie=UTF8&amp;qid=1443805532&amp;sr=1-1&amp;keywords=limit+switch","Limit Switch")</f>
         <v>Limit Switch</v>
@@ -1870,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>85</v>
       </c>
@@ -1880,7 +1974,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009YJ4N6?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Air Pump")</f>
         <v>Air Pump</v>
@@ -1899,8 +1993,11 @@
         <f t="shared" ref="F41:F45" si="8">E41*D41</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G41" s="52" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Jardin-Aquarium-Ceramic-Diffusers-Diameter/dp/B0050HJ7Q6/ref=pd_bxgy_199_img_z","Air Stone")</f>
         <v>Air Stone</v>
@@ -1920,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Standard-Airline-Tubing-Accessories-25-Feet/dp/B0002563MW/ref=pd_bxgy_199_img_y","Air Pump Tubing")</f>
         <v>Air Pump Tubing</v>
@@ -1940,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EWENMAU?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_2&amp;smid=A14L9DIA3NK9B0","Aquarium Pump")</f>
         <v>Aquarium Pump</v>
@@ -1960,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0079QUTSQ?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Pump Tubing")</f>
         <v>Pump Tubing</v>
@@ -1980,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -1990,7 +2087,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1123&amp;search=DFR0300#.VdTDoFNViko","Water Temperature and EC Sensor")</f>
         <v>Water Temperature and EC Sensor</v>
@@ -2010,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1025#.Vg60SBNViko","pH Sensor")</f>
         <v>pH Sensor</v>
@@ -2030,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2040,7 +2137,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00BL63ZU4?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","Cable Management Box")</f>
         <v>Cable Management Box</v>
@@ -2060,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2068,7 +2165,7 @@
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>98</v>
       </c>
@@ -2078,7 +2175,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="str">
         <f>HYPERLINK("C2G / Cables To Go 53408 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (12 Feet/3.65 Meters)","Sacrificial AC Extension Cable for high gauge wire")</f>
         <v>Sacrificial AC Extension Cable for high gauge wire</v>
@@ -2098,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Wago-222-412-222-413-Lever-Nut-Assortment/dp/B00U4520JK/ref=sr_1_1?ie=UTF8&amp;qid=1443798480&amp;sr=8-1&amp;keywords=wago+lever+nut+assortment","Wago Lever Nut Assortment")</f>
         <v>Wago Lever Nut Assortment</v>
@@ -2118,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Vktech-150pcs-Shrink-Tubing-Sleeving/dp/B00EXLPLTW/ref=sr_1_2?ie=UTF8&amp;qid=1440019080&amp;sr=8-2&amp;keywords=vktech+heat+shrink","Heat Shrink Tubing")</f>
         <v>Heat Shrink Tubing</v>
@@ -2138,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-c-98_106_57/?ref=crumb","Grove Cables")</f>
         <v>Grove Cables</v>
@@ -2153,7 +2250,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="8" t="s">
@@ -2163,7 +2260,7 @@
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/3M-Scotch-1-in-x-12-5-yds-Indoor-Outdoor-Mounting-Tape-411-LONG-DC/100153200","Foam mounting tape")</f>
         <v>Foam mounting tape</v>
@@ -2183,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="str">
         <f>HYPERLINK("http://www.amazon.com/3M-Electrical-75-Inch-66-Foot-0085-Inch/dp/B00004WCCP/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1443807012&amp;sr=1-1&amp;keywords=electrical+tape","Electrical Tape")</f>
         <v>Electrical Tape</v>
@@ -2203,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="str">
         <f>HYPERLINK("http://www.digikey.com/product-search/en?KeyWords=377-2132-ND&amp;WT.z_header=search_go","Air Exchange Box")</f>
         <v>Air Exchange Box</v>
@@ -2223,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-6-x-1-2-in-Stainless-Steel-Pan-Head-Phillips-Sheet-Metal-Screw-50-per-Pack-800162/204275035","Short Screws")</f>
         <v>Short Screws</v>
@@ -2243,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-8-x-2-in-Zinc-Plated-Pan-Head-Phillips-Drive-Sheet-Metal-Screw-50-Piece-801632/204275094","Long Screws")</f>
         <v>Long Screws</v>
@@ -2263,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>111</v>
       </c>
@@ -2287,6 +2384,7 @@
     <hyperlink ref="A24" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2298,20 +2396,20 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2340,7 +2438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2357,7 +2455,7 @@
       <c r="G2" s="46"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2384,7 +2482,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2411,7 +2509,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2428,7 +2526,7 @@
       <c r="G5" s="46"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2445,7 +2543,7 @@
       <c r="G6" s="46"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2475,7 +2573,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2505,7 +2603,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2534,7 +2632,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2550,7 +2648,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="46"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2580,7 +2678,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2609,7 +2707,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2626,7 +2724,7 @@
       <c r="G13" s="46"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2656,7 +2754,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2685,7 +2783,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2702,7 +2800,7 @@
       <c r="G16" s="46"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2731,7 +2829,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2758,7 +2856,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2775,7 +2873,7 @@
       <c r="G19" s="46"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2805,7 +2903,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2824,7 +2922,7 @@
       <c r="G21" s="46"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -2839,7 +2937,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2849,7 +2947,7 @@
       <c r="G23" s="19"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2859,7 +2957,7 @@
       <c r="G24" s="19"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2869,35 +2967,35 @@
       <c r="G25" s="19"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" spans="6:7" ht="13" x14ac:dyDescent="0.15">
+    <row r="33" spans="6:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
     </row>
@@ -2920,19 +3018,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2957,7 +3055,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -2984,7 +3082,7 @@
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -3011,7 +3109,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -3038,7 +3136,7 @@
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -3065,7 +3163,7 @@
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -3092,7 +3190,7 @@
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -3119,7 +3217,7 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -3146,7 +3244,7 @@
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -3173,7 +3271,7 @@
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26">
         <v>9</v>
       </c>
@@ -3200,7 +3298,7 @@
       <c r="K10" s="29"/>
       <c r="L10" s="29"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26">
         <v>10</v>
       </c>
@@ -3227,7 +3325,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>11</v>
       </c>
@@ -3254,7 +3352,7 @@
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26">
         <v>12</v>
       </c>
@@ -3281,7 +3379,7 @@
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -3308,7 +3406,7 @@
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -3327,7 +3425,7 @@
       <c r="K15" s="37"/>
       <c r="L15" s="37"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -3341,7 +3439,7 @@
       <c r="K16" s="37"/>
       <c r="L16" s="37"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -3355,7 +3453,7 @@
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -3369,7 +3467,7 @@
       <c r="K18" s="37"/>
       <c r="L18" s="37"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -3411,14 +3509,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
         <v>117</v>
       </c>
@@ -3430,7 +3528,7 @@
       </c>
       <c r="D1" s="40"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>124</v>
       </c>
@@ -3442,7 +3540,7 @@
       </c>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
         <v>127</v>
       </c>
@@ -3454,7 +3552,7 @@
       </c>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
         <v>134</v>
       </c>
@@ -3464,7 +3562,7 @@
       <c r="C4" s="43"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>136</v>
       </c>
@@ -3474,7 +3572,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="40"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>138</v>
       </c>
@@ -3484,7 +3582,7 @@
       <c r="C6" s="43"/>
       <c r="D6" s="40"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>140</v>
       </c>
@@ -3492,7 +3590,7 @@
       <c r="C7" s="43"/>
       <c r="D7" s="40"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>141</v>
       </c>
@@ -3500,7 +3598,7 @@
       <c r="C8" s="43"/>
       <c r="D8" s="40"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>142</v>
       </c>
@@ -3508,7 +3606,7 @@
       <c r="C9" s="43"/>
       <c r="D9" s="40"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
         <v>143</v>
       </c>
@@ -3516,7 +3614,7 @@
       <c r="C10" s="43"/>
       <c r="D10" s="40"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
         <v>144</v>
       </c>
@@ -3524,7 +3622,7 @@
       <c r="C11" s="43"/>
       <c r="D11" s="40"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
         <v>145</v>
       </c>
@@ -3532,7 +3630,7 @@
       <c r="C12" s="43"/>
       <c r="D12" s="40"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="41" t="s">
         <v>146</v>
       </c>
@@ -3540,7 +3638,7 @@
       <c r="C13" s="43"/>
       <c r="D13" s="40"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
         <v>147</v>
       </c>
@@ -3548,7 +3646,7 @@
       <c r="C14" s="43"/>
       <c r="D14" s="40"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
         <v>148</v>
       </c>
@@ -3556,7 +3654,7 @@
       <c r="C15" s="43"/>
       <c r="D15" s="40"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
         <v>149</v>
       </c>
@@ -3564,7 +3662,7 @@
       <c r="C16" s="43"/>
       <c r="D16" s="40"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
         <v>150</v>
       </c>
@@ -3572,7 +3670,7 @@
       <c r="C17" s="43"/>
       <c r="D17" s="40"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
         <v>151</v>
       </c>
@@ -3580,7 +3678,7 @@
       <c r="C18" s="43"/>
       <c r="D18" s="40"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
         <v>152</v>
       </c>
@@ -3588,7 +3686,7 @@
       <c r="C19" s="43"/>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="s">
         <v>153</v>
       </c>
@@ -3596,7 +3694,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="40"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41" t="s">
         <v>154</v>
       </c>
@@ -3604,7 +3702,7 @@
       <c r="C21" s="43"/>
       <c r="D21" s="40"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41" t="s">
         <v>155</v>
       </c>
@@ -3612,7 +3710,7 @@
       <c r="C22" s="43"/>
       <c r="D22" s="40"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41" t="s">
         <v>156</v>
       </c>
@@ -3620,7 +3718,7 @@
       <c r="C23" s="43"/>
       <c r="D23" s="40"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41" t="s">
         <v>158</v>
       </c>
@@ -3628,7 +3726,7 @@
       <c r="C24" s="43"/>
       <c r="D24" s="40"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
         <v>160</v>
       </c>
@@ -3636,27 +3734,27 @@
       <c r="C25" s="43"/>
       <c r="D25" s="40"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>

</xml_diff>

<commit_message>
Bought more stuff :)
Also added a line for the Aluminium tape that’s not included in the BOM
but referenced in the instructions.
</commit_message>
<xml_diff>
--- a/BOM food computer (New Zealand).xlsx
+++ b/BOM food computer (New Zealand).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raycooke/Documents/Projects/FoodComputer/gro-hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Motherboard" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,20 @@
     <sheet name="Kit" sheetId="3" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="204">
   <si>
     <t>Item Name</t>
   </si>
@@ -633,12 +636,18 @@
   </si>
   <si>
     <t>Ash</t>
+  </si>
+  <si>
+    <t>Aluminium Tape</t>
+  </si>
+  <si>
+    <t>for joins in jacket foam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1167,21 +1176,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1213,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1215,7 +1224,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="48"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CyberPower-CSB606-Protector-6-Outlets-Joules/dp/B00FLTTGYG/ref=pd_sim_23_1?ie=UTF8&amp;refRID=163NC2W6A2KW7EF2RB9B","Power Strip")</f>
         <v>Power Strip</v>
@@ -1238,7 +1247,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Switching-Power-Supply-Strip-Light/dp/B007MWNF5Q/ref=pd_sim_60_6?ie=UTF8&amp;refRID=0WA6QTYVKRWRGRG1ZKN2A","Main Power Supply")</f>
         <v>Main Power Supply</v>
@@ -1261,7 +1270,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0002J1KS0/ref=ox_sc_act_title_1?ie=UTF8&amp;psc=1&amp;smid=ATVPDKIKX0DER","AC Extension Cable")</f>
         <v>AC Extension Cable</v>
@@ -1284,7 +1293,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1304,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="48"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/CanaKit-Raspberry-Power-Supply-Listed/dp/B00MARDJZ4/ref=sr_1_2?ie=UTF8&amp;qid=1439988175&amp;sr=8-2&amp;keywords=raspberry+pi+2+power+supply","Raspberry Pi Power Supply")</f>
         <v>Raspberry Pi Power Supply</v>
@@ -1318,7 +1327,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Ximico-Arduino-Cable-Atmega2560-16au-Compatible/dp/B00KG3SBE8/ref=sr_1_2?s=pc&amp;ie=UTF8&amp;qid=1439935660&amp;sr=1-2&amp;keywords=arduino+mega","Arduino Mega 2560")</f>
         <v>Arduino Mega 2560</v>
@@ -1341,7 +1350,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Raspberry-Pi-Model-Desktop-Linux/dp/B00T2U7R7I","Raspberry Pi 2 Model B")</f>
         <v>Raspberry Pi 2 Model B</v>
@@ -1364,7 +1373,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_8?s=pc&amp;ie=UTF8&amp;qid=1439988385&amp;sr=1-8&amp;keywords=micro+SD","Micro SD Card")</f>
         <v>Micro SD Card</v>
@@ -1387,7 +1396,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EUHRLF6/ref=ox_sc_imb_mini_detail?ie=UTF8&amp;psc=1&amp;smid=A1DCPNQKKEISZB","Ethernet cable")</f>
         <v>Ethernet cable</v>
@@ -1408,7 +1417,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Gikfun-Protoshield-Prototype-Shield-Arduino/dp/B00Q9YBQ04/ref=sr_1_6?s=pc&amp;ie=UTF8&amp;qid=1439935499&amp;sr=1-6&amp;keywords=protoshield","Arduino Mega Protoshield")</f>
         <v>Arduino Mega Protoshield</v>
@@ -1431,7 +1440,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Base-Shield-V2-p-1378.html","Grove Base Shield")</f>
         <v>Grove Base Shield</v>
@@ -1454,7 +1463,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="str">
         <f>HYPERLINK("https://www.adafruit.com/products/2097","Touchscreen Display")</f>
         <v>Touchscreen Display</v>
@@ -1477,7 +1486,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/ribbon-cable-Raspberry-stackable-header/dp/B00G84WNA2/ref=sr_1_1?ie=UTF8&amp;qid=1440708449&amp;sr=8-1&amp;keywords=raspberry+pi+cable","GPIO Cable ")</f>
         <v xml:space="preserve">GPIO Cable </v>
@@ -1500,7 +1509,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -1510,7 +1519,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/JBtek-Channel-Module-Arduino-Raspberry/dp/B00KTEN3TM/ref=sr_1_1?s=pc&amp;ie=UTF8&amp;qid=1439935182&amp;sr=1-1&amp;keywords=4+Channel+Relay","4-Channel Relay")</f>
         <v>4-Channel Relay</v>
@@ -1533,7 +1542,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/52171-4E-Pre-Galvanized-Eccentric-Knockouts/dp/B000HEFCKC/ref=pd_bxgy_60_text_y","AC Relay Box Back Receptacle")</f>
         <v>AC Relay Box Back Receptacle</v>
@@ -1556,7 +1565,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/RS8-Outlet-Surface-Square-Galvanized/dp/B000HEIU9W/ref=pd_sim_60_23?ie=UTF8&amp;refRID=0C95J370DWVEWW0H1MG8","AC Relay Box Front Panel")</f>
         <v>AC Relay Box Front Panel</v>
@@ -1579,7 +1588,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>199</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>198</v>
       </c>
@@ -1623,7 +1632,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -1633,7 +1642,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>197</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="47" t="s">
         <v>196</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
@@ -1689,7 +1698,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B003XDTWN2/ref=sr_ph?&amp;ie=UTF8&amp;qid=1440085101&amp;sr=1&amp;keywords=heater","Heater")</f>
         <v>Heater</v>
@@ -1712,7 +1721,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Acoustic-Audio-Tek%C2%A8Portable-Humidifier-travel--White/dp/B00RM5Z44S/ref=sr_1_4?s=home-garden&amp;ie=UTF8&amp;qid=1440427700&amp;sr=1-4&amp;keywords=bottle+cap+humidifier","Humidifier")</f>
         <v>Humidifier</v>
@@ -1735,7 +1744,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/dp/B00WJW3NM4/ref=twister_B00WJW3M3Y?_encoding=UTF8&amp;psc=1","USB Wall Adapter")</f>
         <v>USB Wall Adapter</v>
@@ -1755,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Bgears-b-Blaster-120mm-Bearing-Extreme/dp/B0043GKY1W/ref=sr_1_1?ie=UTF8&amp;qid=1440020490&amp;sr=8-1&amp;keywords=bgears+120mm","Circulation/Vent Fans")</f>
         <v>Circulation/Vent Fans</v>
@@ -1778,7 +1787,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Tjernlund-1519003-Wire-Fan-Guard/dp/B008RMKFTO/ref=sr_1_2?ie=UTF8&amp;qid=1440019946&amp;sr=8-2&amp;keywords=fan+guard","Fan Guards")</f>
         <v>Fan Guards</v>
@@ -1801,7 +1810,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Dundas-Jafine-LC4WZW-ProVent-4-Inches/dp/B0016487CC/ref=sr_1_3?ie=UTF8&amp;qid=1440020385&amp;sr=8-3&amp;keywords=Louvered+Vent+Cap","Fan Louvres")</f>
         <v>Fan Louvres</v>
@@ -1824,7 +1833,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
@@ -1834,7 +1843,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="str">
         <f>HYPERLINK("http://www.co2meter.com/products/cozir-0-2-co2-sensor","CO2 Sensor")</f>
         <v>CO2 Sensor</v>
@@ -1854,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-TemperatureHumidity-Sensor-Pro-p-838.html","Air Temperature and Humidity Sensor")</f>
         <v>Air Temperature and Humidity Sensor</v>
@@ -1874,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-Digital-Light-Sensor-p-1281.html","Light Intensity Sensor")</f>
         <v>Light Intensity Sensor</v>
@@ -1894,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00YCDHQ8K?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o06_s00","Webcam")</f>
         <v>Webcam</v>
@@ -1914,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
@@ -1924,7 +1933,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009SUF08?keywords=reed%20switch&amp;qid=1443805349&amp;ref_=sr_1_1&amp;sr=8-1","Magnetic Switch")</f>
         <v>Magnetic Switch</v>
@@ -1944,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Micro-Limit-Switch-Roller-Action/dp/B00E0JOTV8/ref=sr_1_1?s=lamps-light&amp;ie=UTF8&amp;qid=1443805532&amp;sr=1-1&amp;keywords=limit+switch","Limit Switch")</f>
         <v>Limit Switch</v>
@@ -1964,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>85</v>
       </c>
@@ -1974,7 +1983,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0009YJ4N6?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Air Pump")</f>
         <v>Air Pump</v>
@@ -1997,7 +2006,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Jardin-Aquarium-Ceramic-Diffusers-Diameter/dp/B0050HJ7Q6/ref=pd_bxgy_199_img_z","Air Stone")</f>
         <v>Air Stone</v>
@@ -2017,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Standard-Airline-Tubing-Accessories-25-Feet/dp/B0002563MW/ref=pd_bxgy_199_img_y","Air Pump Tubing")</f>
         <v>Air Pump Tubing</v>
@@ -2037,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00EWENMAU?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_2&amp;smid=A14L9DIA3NK9B0","Aquarium Pump")</f>
         <v>Aquarium Pump</v>
@@ -2057,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B0079QUTSQ?psc=1&amp;redirect=true&amp;ref_=ox_sc_act_title_1&amp;smid=ATVPDKIKX0DER","Pump Tubing")</f>
         <v>Pump Tubing</v>
@@ -2077,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -2087,7 +2096,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1123&amp;search=DFR0300#.VdTDoFNViko","Water Temperature and EC Sensor")</f>
         <v>Water Temperature and EC Sensor</v>
@@ -2107,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="str">
         <f>HYPERLINK("http://www.dfrobot.com/index.php?route=product/product&amp;product_id=1025#.Vg60SBNViko","pH Sensor")</f>
         <v>pH Sensor</v>
@@ -2127,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2137,7 +2146,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/gp/product/B00BL63ZU4?psc=1&amp;redirect=true&amp;ref_=oh_aui_detailpage_o01_s00","Cable Management Box")</f>
         <v>Cable Management Box</v>
@@ -2157,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2165,7 +2174,7 @@
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>98</v>
       </c>
@@ -2175,7 +2184,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="str">
         <f>HYPERLINK("C2G / Cables To Go 53408 18 AWG Outlet Saver Power Extension Cord for NEMA 5-15P to NEMA 5-15R, Black (12 Feet/3.65 Meters)","Sacrificial AC Extension Cable for high gauge wire")</f>
         <v>Sacrificial AC Extension Cable for high gauge wire</v>
@@ -2195,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Wago-222-412-222-413-Lever-Nut-Assortment/dp/B00U4520JK/ref=sr_1_1?ie=UTF8&amp;qid=1443798480&amp;sr=8-1&amp;keywords=wago+lever+nut+assortment","Wago Lever Nut Assortment")</f>
         <v>Wago Lever Nut Assortment</v>
@@ -2215,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="str">
         <f>HYPERLINK("http://www.amazon.com/Vktech-150pcs-Shrink-Tubing-Sleeving/dp/B00EXLPLTW/ref=sr_1_2?ie=UTF8&amp;qid=1440019080&amp;sr=8-2&amp;keywords=vktech+heat+shrink","Heat Shrink Tubing")</f>
         <v>Heat Shrink Tubing</v>
@@ -2235,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="str">
         <f>HYPERLINK("http://www.seeedstudio.com/depot/Grove-c-98_106_57/?ref=crumb","Grove Cables")</f>
         <v>Grove Cables</v>
@@ -2250,7 +2259,7 @@
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="8" t="s">
@@ -2260,7 +2269,7 @@
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/3M-Scotch-1-in-x-12-5-yds-Indoor-Outdoor-Mounting-Tape-411-LONG-DC/100153200","Foam mounting tape")</f>
         <v>Foam mounting tape</v>
@@ -2280,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="22" t="str">
         <f>HYPERLINK("http://www.amazon.com/3M-Electrical-75-Inch-66-Foot-0085-Inch/dp/B00004WCCP/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1443807012&amp;sr=1-1&amp;keywords=electrical+tape","Electrical Tape")</f>
         <v>Electrical Tape</v>
@@ -2300,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="22" t="str">
         <f>HYPERLINK("http://www.digikey.com/product-search/en?KeyWords=377-2132-ND&amp;WT.z_header=search_go","Air Exchange Box")</f>
         <v>Air Exchange Box</v>
@@ -2320,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-6-x-1-2-in-Stainless-Steel-Pan-Head-Phillips-Sheet-Metal-Screw-50-per-Pack-800162/204275035","Short Screws")</f>
         <v>Short Screws</v>
@@ -2340,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="22" t="str">
         <f>HYPERLINK("http://www.homedepot.com/p/Everbilt-8-x-2-in-Zinc-Plated-Pan-Head-Phillips-Drive-Sheet-Metal-Screw-50-Piece-801632/204275094","Long Screws")</f>
         <v>Long Screws</v>
@@ -2360,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>111</v>
       </c>
@@ -2393,23 +2402,23 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="181" zoomScalePageLayoutView="181" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="77.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2438,7 +2447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2455,7 +2464,7 @@
       <c r="G2" s="46"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2482,7 +2491,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2509,7 +2518,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2522,11 +2531,22 @@
       <c r="D5" s="4">
         <v>6</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="46"/>
+      <c r="E5" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="46">
+        <f>2.97*6</f>
+        <v>17.82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>180</v>
+      </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2543,7 +2563,7 @@
       <c r="G6" s="46"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2573,7 +2593,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2603,7 +2623,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2632,7 +2652,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2645,10 +2665,20 @@
       <c r="D10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="46">
+        <v>13.24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2678,7 +2708,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2707,7 +2737,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2724,7 +2754,7 @@
       <c r="G13" s="46"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2754,7 +2784,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2783,7 +2813,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2800,7 +2830,7 @@
       <c r="G16" s="46"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2829,7 +2859,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2856,7 +2886,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2873,7 +2903,7 @@
       <c r="G19" s="46"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2903,7 +2933,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2916,38 +2946,66 @@
       <c r="D21" s="4">
         <v>2</v>
       </c>
+      <c r="E21" t="s">
+        <v>178</v>
+      </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="4" t="s">
-        <v>52</v>
+      <c r="G21" s="46">
+        <f>9.21</f>
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="H21" t="s">
+        <v>180</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="18">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" s="18">
+        <v>1</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="F22" s="18">
+        <v>1</v>
       </c>
       <c r="G22" s="46">
-        <f>SUM(G2:G21)</f>
-        <v>236.37999999999997</v>
+        <v>10.23</v>
+      </c>
+      <c r="H22" t="s">
+        <v>180</v>
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
+      <c r="F23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="46">
+        <f>SUM(G2:G22)</f>
+        <v>286.87999999999994</v>
+      </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2957,7 +3015,7 @@
       <c r="G24" s="19"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2967,35 +3025,35 @@
       <c r="G25" s="19"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" spans="6:7" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:7" ht="13" x14ac:dyDescent="0.15">
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
     </row>
@@ -3005,6 +3063,9 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E18" r:id="rId3"/>
     <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="E22" r:id="rId6"/>
+    <hyperlink ref="E5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3018,19 +3079,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3055,7 +3116,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -3082,7 +3143,7 @@
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -3109,7 +3170,7 @@
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -3136,7 +3197,7 @@
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -3163,7 +3224,7 @@
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -3190,7 +3251,7 @@
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -3217,7 +3278,7 @@
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -3244,7 +3305,7 @@
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -3271,7 +3332,7 @@
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="26">
         <v>9</v>
       </c>
@@ -3298,7 +3359,7 @@
       <c r="K10" s="29"/>
       <c r="L10" s="29"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="26">
         <v>10</v>
       </c>
@@ -3325,7 +3386,7 @@
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="26">
         <v>11</v>
       </c>
@@ -3352,7 +3413,7 @@
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="26">
         <v>12</v>
       </c>
@@ -3379,7 +3440,7 @@
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="34">
         <v>13</v>
       </c>
@@ -3406,7 +3467,7 @@
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="37"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -3425,7 +3486,7 @@
       <c r="K15" s="37"/>
       <c r="L15" s="37"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="37"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -3439,7 +3500,7 @@
       <c r="K16" s="37"/>
       <c r="L16" s="37"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="37"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -3453,7 +3514,7 @@
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="37"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -3467,7 +3528,7 @@
       <c r="K18" s="37"/>
       <c r="L18" s="37"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="37"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -3509,14 +3570,14 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="39" t="s">
         <v>117</v>
       </c>
@@ -3528,7 +3589,7 @@
       </c>
       <c r="D1" s="40"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="41" t="s">
         <v>124</v>
       </c>
@@ -3540,7 +3601,7 @@
       </c>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="42" t="s">
         <v>127</v>
       </c>
@@ -3552,7 +3613,7 @@
       </c>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="41" t="s">
         <v>134</v>
       </c>
@@ -3562,7 +3623,7 @@
       <c r="C4" s="43"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="41" t="s">
         <v>136</v>
       </c>
@@ -3572,7 +3633,7 @@
       <c r="C5" s="43"/>
       <c r="D5" s="40"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="41" t="s">
         <v>138</v>
       </c>
@@ -3582,7 +3643,7 @@
       <c r="C6" s="43"/>
       <c r="D6" s="40"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="41" t="s">
         <v>140</v>
       </c>
@@ -3590,7 +3651,7 @@
       <c r="C7" s="43"/>
       <c r="D7" s="40"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="41" t="s">
         <v>141</v>
       </c>
@@ -3598,7 +3659,7 @@
       <c r="C8" s="43"/>
       <c r="D8" s="40"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="41" t="s">
         <v>142</v>
       </c>
@@ -3606,7 +3667,7 @@
       <c r="C9" s="43"/>
       <c r="D9" s="40"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="41" t="s">
         <v>143</v>
       </c>
@@ -3614,7 +3675,7 @@
       <c r="C10" s="43"/>
       <c r="D10" s="40"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="41" t="s">
         <v>144</v>
       </c>
@@ -3622,7 +3683,7 @@
       <c r="C11" s="43"/>
       <c r="D11" s="40"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="41" t="s">
         <v>145</v>
       </c>
@@ -3630,7 +3691,7 @@
       <c r="C12" s="43"/>
       <c r="D12" s="40"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="41" t="s">
         <v>146</v>
       </c>
@@ -3638,7 +3699,7 @@
       <c r="C13" s="43"/>
       <c r="D13" s="40"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="41" t="s">
         <v>147</v>
       </c>
@@ -3646,7 +3707,7 @@
       <c r="C14" s="43"/>
       <c r="D14" s="40"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="41" t="s">
         <v>148</v>
       </c>
@@ -3654,7 +3715,7 @@
       <c r="C15" s="43"/>
       <c r="D15" s="40"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="41" t="s">
         <v>149</v>
       </c>
@@ -3662,7 +3723,7 @@
       <c r="C16" s="43"/>
       <c r="D16" s="40"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="41" t="s">
         <v>150</v>
       </c>
@@ -3670,7 +3731,7 @@
       <c r="C17" s="43"/>
       <c r="D17" s="40"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="41" t="s">
         <v>151</v>
       </c>
@@ -3678,7 +3739,7 @@
       <c r="C18" s="43"/>
       <c r="D18" s="40"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="41" t="s">
         <v>152</v>
       </c>
@@ -3686,7 +3747,7 @@
       <c r="C19" s="43"/>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="41" t="s">
         <v>153</v>
       </c>
@@ -3694,7 +3755,7 @@
       <c r="C20" s="43"/>
       <c r="D20" s="40"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="41" t="s">
         <v>154</v>
       </c>
@@ -3702,7 +3763,7 @@
       <c r="C21" s="43"/>
       <c r="D21" s="40"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="41" t="s">
         <v>155</v>
       </c>
@@ -3710,7 +3771,7 @@
       <c r="C22" s="43"/>
       <c r="D22" s="40"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="41" t="s">
         <v>156</v>
       </c>
@@ -3718,7 +3779,7 @@
       <c r="C23" s="43"/>
       <c r="D23" s="40"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="41" t="s">
         <v>158</v>
       </c>
@@ -3726,7 +3787,7 @@
       <c r="C24" s="43"/>
       <c r="D24" s="40"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="41" t="s">
         <v>160</v>
       </c>
@@ -3734,27 +3795,27 @@
       <c r="C25" s="43"/>
       <c r="D25" s="40"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="10"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>

</xml_diff>